<commit_message>
SQL about the latest basic data update By Richard 20160112
</commit_message>
<xml_diff>
--- a/03_Database/Basic Data.xlsx
+++ b/03_Database/Basic Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="195" windowWidth="14805" windowHeight="7920"/>
   </bookViews>
   <sheets>
     <sheet name="商品分类定义" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="636">
   <si>
     <t>classId</t>
   </si>
@@ -1707,6 +1707,291 @@
   <si>
     <t>2020-01-01 00:00:00</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>GD20160201000001</t>
+  </si>
+  <si>
+    <t>GD20160201000002</t>
+  </si>
+  <si>
+    <t>GD20160201000003</t>
+  </si>
+  <si>
+    <t>GD20160201000004</t>
+  </si>
+  <si>
+    <t>GD20160201000005</t>
+  </si>
+  <si>
+    <t>GD20160201000006</t>
+  </si>
+  <si>
+    <t>GD20160201000007</t>
+  </si>
+  <si>
+    <t>GD20160201000008</t>
+  </si>
+  <si>
+    <t>GD20160201000009</t>
+  </si>
+  <si>
+    <t>GD20160201000010</t>
+  </si>
+  <si>
+    <t>GD20160201000011</t>
+  </si>
+  <si>
+    <t>GD20160201000012</t>
+  </si>
+  <si>
+    <t>GD20160201000013</t>
+  </si>
+  <si>
+    <t>GD20160201000014</t>
+  </si>
+  <si>
+    <t>GD20160201000015</t>
+  </si>
+  <si>
+    <t>GD20160201000016</t>
+  </si>
+  <si>
+    <t>GD20160201000017</t>
+  </si>
+  <si>
+    <t>GD20160201000018</t>
+  </si>
+  <si>
+    <t>GD20160201000019</t>
+  </si>
+  <si>
+    <t>GD20160201000020</t>
+  </si>
+  <si>
+    <t>GD20160201000021</t>
+  </si>
+  <si>
+    <t>GD20160201000022</t>
+  </si>
+  <si>
+    <t>GD20160201000023</t>
+  </si>
+  <si>
+    <t>GD20160201000024</t>
+  </si>
+  <si>
+    <t>GD20160201000025</t>
+  </si>
+  <si>
+    <t>GD20160201000026</t>
+  </si>
+  <si>
+    <t>GD20160201000027</t>
+  </si>
+  <si>
+    <t>GD20160201000028</t>
+  </si>
+  <si>
+    <t>GD20160201000029</t>
+  </si>
+  <si>
+    <t>GD20160201000030</t>
+  </si>
+  <si>
+    <t>GD20160201000031</t>
+  </si>
+  <si>
+    <t>GD20160201000032</t>
+  </si>
+  <si>
+    <t>GD20160201000033</t>
+  </si>
+  <si>
+    <t>GD20160201000034</t>
+  </si>
+  <si>
+    <t>GD20160201000035</t>
+  </si>
+  <si>
+    <t>GD20160201000036</t>
+  </si>
+  <si>
+    <t>GD20160201000037</t>
+  </si>
+  <si>
+    <t>GD20160201000038</t>
+  </si>
+  <si>
+    <t>GD20160201000039</t>
+  </si>
+  <si>
+    <t>GD20160201000040</t>
+  </si>
+  <si>
+    <t>GD20160201000041</t>
+  </si>
+  <si>
+    <t>GD20160201000042</t>
+  </si>
+  <si>
+    <t>GD20160201000043</t>
+  </si>
+  <si>
+    <t>GD20160201000044</t>
+  </si>
+  <si>
+    <t>GD20160201000045</t>
+  </si>
+  <si>
+    <t>GD20160201000046</t>
+  </si>
+  <si>
+    <t>GD20160201000047</t>
+  </si>
+  <si>
+    <t>GD20160201000048</t>
+  </si>
+  <si>
+    <t>GD20160201000049</t>
+  </si>
+  <si>
+    <t>GD20160201000050</t>
+  </si>
+  <si>
+    <t>GD20160201000051</t>
+  </si>
+  <si>
+    <t>GD20160201000052</t>
+  </si>
+  <si>
+    <t>GD20160201000053</t>
+  </si>
+  <si>
+    <t>GD20160201000054</t>
+  </si>
+  <si>
+    <t>GD20160201000055</t>
+  </si>
+  <si>
+    <t>GD20160201000056</t>
+  </si>
+  <si>
+    <t>GD20160201000057</t>
+  </si>
+  <si>
+    <t>GD20160201000058</t>
+  </si>
+  <si>
+    <t>GD20160201000059</t>
+  </si>
+  <si>
+    <t>GD20160201000060</t>
+  </si>
+  <si>
+    <t>GD20160201000061</t>
+  </si>
+  <si>
+    <t>GD20160201000062</t>
+  </si>
+  <si>
+    <t>GD20160201000063</t>
+  </si>
+  <si>
+    <t>GD20160201000064</t>
+  </si>
+  <si>
+    <t>GD20160201000065</t>
+  </si>
+  <si>
+    <t>GD20160201000066</t>
+  </si>
+  <si>
+    <t>GD20160201000067</t>
+  </si>
+  <si>
+    <t>GD20160201000068</t>
+  </si>
+  <si>
+    <t>GD20160201000069</t>
+  </si>
+  <si>
+    <t>GD20160201000070</t>
+  </si>
+  <si>
+    <t>GD20160201000071</t>
+  </si>
+  <si>
+    <t>GD20160201000072</t>
+  </si>
+  <si>
+    <t>GD20160201000073</t>
+  </si>
+  <si>
+    <t>GD20160201000074</t>
+  </si>
+  <si>
+    <t>GD20160201000075</t>
+  </si>
+  <si>
+    <t>GD20160201000076</t>
+  </si>
+  <si>
+    <t>GD20160201000077</t>
+  </si>
+  <si>
+    <t>GD20160201000078</t>
+  </si>
+  <si>
+    <t>GD20160201000079</t>
+  </si>
+  <si>
+    <t>GD20160201000080</t>
+  </si>
+  <si>
+    <t>GD20160201000081</t>
+  </si>
+  <si>
+    <t>GD20160201000082</t>
+  </si>
+  <si>
+    <t>GD20160201000083</t>
+  </si>
+  <si>
+    <t>GD20160201000084</t>
+  </si>
+  <si>
+    <t>GD20160201000085</t>
+  </si>
+  <si>
+    <t>GD20160201000086</t>
+  </si>
+  <si>
+    <t>GD20160201000087</t>
+  </si>
+  <si>
+    <t>GD20160201000088</t>
+  </si>
+  <si>
+    <t>GD20160201000089</t>
+  </si>
+  <si>
+    <t>GD20160201000090</t>
+  </si>
+  <si>
+    <t>GD20160201000091</t>
+  </si>
+  <si>
+    <t>GD20160201000092</t>
+  </si>
+  <si>
+    <t>GD20160201000093</t>
+  </si>
+  <si>
+    <t>GD20160201000094</t>
+  </si>
+  <si>
+    <t>GD20160201000095</t>
   </si>
 </sst>
 </file>
@@ -1816,8 +2101,36 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3265,7 +3578,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B3" s="6" t="s">
-        <v>212</v>
+        <v>541</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>59</v>
@@ -3317,7 +3630,7 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B4" s="6" t="s">
-        <v>213</v>
+        <v>542</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>59</v>
@@ -3369,7 +3682,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B5" s="6" t="s">
-        <v>214</v>
+        <v>543</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>59</v>
@@ -3421,7 +3734,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B6" s="6" t="s">
-        <v>215</v>
+        <v>544</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>54</v>
@@ -3473,7 +3786,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B7" s="6" t="s">
-        <v>216</v>
+        <v>545</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>56</v>
@@ -3525,7 +3838,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B8" s="6" t="s">
-        <v>217</v>
+        <v>546</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>48</v>
@@ -3577,7 +3890,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B9" s="6" t="s">
-        <v>218</v>
+        <v>547</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>48</v>
@@ -3629,7 +3942,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B10" s="6" t="s">
-        <v>219</v>
+        <v>548</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>48</v>
@@ -3681,7 +3994,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B11" s="6" t="s">
-        <v>220</v>
+        <v>549</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>48</v>
@@ -3733,7 +4046,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B12" s="6" t="s">
-        <v>221</v>
+        <v>550</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>55</v>
@@ -3785,7 +4098,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B13" s="6" t="s">
-        <v>222</v>
+        <v>551</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>61</v>
@@ -3837,7 +4150,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B14" s="6" t="s">
-        <v>223</v>
+        <v>552</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>63</v>
@@ -3889,7 +4202,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B15" s="6" t="s">
-        <v>224</v>
+        <v>553</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>61</v>
@@ -3941,7 +4254,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.15">
       <c r="B16" s="6" t="s">
-        <v>225</v>
+        <v>554</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>48</v>
@@ -3993,7 +4306,7 @@
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B17" s="6" t="s">
-        <v>226</v>
+        <v>555</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>48</v>
@@ -4045,7 +4358,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B18" s="6" t="s">
-        <v>227</v>
+        <v>556</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>48</v>
@@ -4097,7 +4410,7 @@
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B19" s="6" t="s">
-        <v>228</v>
+        <v>557</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>58</v>
@@ -4149,7 +4462,7 @@
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B20" s="6" t="s">
-        <v>229</v>
+        <v>558</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>59</v>
@@ -4201,7 +4514,7 @@
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B21" s="6" t="s">
-        <v>230</v>
+        <v>559</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>59</v>
@@ -4253,7 +4566,7 @@
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B22" s="6" t="s">
-        <v>231</v>
+        <v>560</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>63</v>
@@ -4305,7 +4618,7 @@
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B23" s="6" t="s">
-        <v>232</v>
+        <v>561</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>63</v>
@@ -4357,7 +4670,7 @@
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B24" s="6" t="s">
-        <v>233</v>
+        <v>562</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>63</v>
@@ -4409,7 +4722,7 @@
     </row>
     <row r="25" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B25" s="6" t="s">
-        <v>234</v>
+        <v>563</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>65</v>
@@ -4461,7 +4774,7 @@
     </row>
     <row r="26" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B26" s="6" t="s">
-        <v>235</v>
+        <v>564</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>55</v>
@@ -4513,7 +4826,7 @@
     </row>
     <row r="27" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B27" s="6" t="s">
-        <v>236</v>
+        <v>565</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>48</v>
@@ -4565,7 +4878,7 @@
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B28" s="6" t="s">
-        <v>237</v>
+        <v>566</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>48</v>
@@ -4617,7 +4930,7 @@
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B29" s="6" t="s">
-        <v>238</v>
+        <v>567</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>63</v>
@@ -4669,7 +4982,7 @@
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B30" s="6" t="s">
-        <v>239</v>
+        <v>568</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>65</v>
@@ -4721,7 +5034,7 @@
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B31" s="6" t="s">
-        <v>240</v>
+        <v>569</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>65</v>
@@ -4773,7 +5086,7 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B32" s="6" t="s">
-        <v>241</v>
+        <v>570</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>65</v>
@@ -4825,7 +5138,7 @@
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B33" s="6" t="s">
-        <v>242</v>
+        <v>571</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>63</v>
@@ -4877,7 +5190,7 @@
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B34" s="6" t="s">
-        <v>243</v>
+        <v>572</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>48</v>
@@ -4929,7 +5242,7 @@
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
-        <v>244</v>
+        <v>573</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>58</v>
@@ -4981,7 +5294,7 @@
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B36" s="6" t="s">
-        <v>245</v>
+        <v>574</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>48</v>
@@ -5033,7 +5346,7 @@
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B37" s="6" t="s">
-        <v>246</v>
+        <v>575</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>50</v>
@@ -5085,7 +5398,7 @@
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B38" s="6" t="s">
-        <v>247</v>
+        <v>576</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>58</v>
@@ -5137,7 +5450,7 @@
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B39" s="6" t="s">
-        <v>248</v>
+        <v>577</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>58</v>
@@ -5189,7 +5502,7 @@
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B40" s="6" t="s">
-        <v>249</v>
+        <v>578</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>58</v>
@@ -5241,7 +5554,7 @@
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B41" s="6" t="s">
-        <v>250</v>
+        <v>579</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>58</v>
@@ -5293,7 +5606,7 @@
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B42" s="6" t="s">
-        <v>251</v>
+        <v>580</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>48</v>
@@ -5345,7 +5658,7 @@
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B43" s="6" t="s">
-        <v>252</v>
+        <v>581</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>48</v>
@@ -5397,7 +5710,7 @@
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B44" s="6" t="s">
-        <v>253</v>
+        <v>582</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>48</v>
@@ -5449,7 +5762,7 @@
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B45" s="6" t="s">
-        <v>254</v>
+        <v>583</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>48</v>
@@ -5501,7 +5814,7 @@
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B46" s="6" t="s">
-        <v>255</v>
+        <v>584</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>48</v>
@@ -5553,7 +5866,7 @@
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B47" s="6" t="s">
-        <v>256</v>
+        <v>585</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>55</v>
@@ -5605,7 +5918,7 @@
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B48" s="6" t="s">
-        <v>257</v>
+        <v>586</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>56</v>
@@ -5657,7 +5970,7 @@
     </row>
     <row r="49" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B49" s="6" t="s">
-        <v>258</v>
+        <v>587</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>65</v>
@@ -5709,7 +6022,7 @@
     </row>
     <row r="50" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B50" s="6" t="s">
-        <v>259</v>
+        <v>588</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>48</v>
@@ -5761,7 +6074,7 @@
     </row>
     <row r="51" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B51" s="6" t="s">
-        <v>260</v>
+        <v>589</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>48</v>
@@ -5813,7 +6126,7 @@
     </row>
     <row r="52" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B52" s="6" t="s">
-        <v>261</v>
+        <v>590</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>48</v>
@@ -5865,7 +6178,7 @@
     </row>
     <row r="53" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B53" s="6" t="s">
-        <v>262</v>
+        <v>591</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>55</v>
@@ -5917,7 +6230,7 @@
     </row>
     <row r="54" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B54" s="6" t="s">
-        <v>263</v>
+        <v>592</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>56</v>
@@ -5969,7 +6282,7 @@
     </row>
     <row r="55" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B55" s="6" t="s">
-        <v>264</v>
+        <v>593</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>56</v>
@@ -6021,7 +6334,7 @@
     </row>
     <row r="56" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B56" s="6" t="s">
-        <v>265</v>
+        <v>594</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>55</v>
@@ -6073,7 +6386,7 @@
     </row>
     <row r="57" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B57" s="6" t="s">
-        <v>266</v>
+        <v>595</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>50</v>
@@ -6125,7 +6438,7 @@
     </row>
     <row r="58" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B58" s="6" t="s">
-        <v>267</v>
+        <v>596</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>56</v>
@@ -6177,7 +6490,7 @@
     </row>
     <row r="59" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B59" s="6" t="s">
-        <v>268</v>
+        <v>597</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>48</v>
@@ -6229,7 +6542,7 @@
     </row>
     <row r="60" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B60" s="6" t="s">
-        <v>269</v>
+        <v>598</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>48</v>
@@ -6281,7 +6594,7 @@
     </row>
     <row r="61" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B61" s="6" t="s">
-        <v>270</v>
+        <v>599</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>48</v>
@@ -6333,7 +6646,7 @@
     </row>
     <row r="62" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B62" s="6" t="s">
-        <v>271</v>
+        <v>600</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>48</v>
@@ -6385,7 +6698,7 @@
     </row>
     <row r="63" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B63" s="6" t="s">
-        <v>272</v>
+        <v>601</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>48</v>
@@ -6437,7 +6750,7 @@
     </row>
     <row r="64" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B64" s="6" t="s">
-        <v>273</v>
+        <v>602</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>48</v>
@@ -6489,7 +6802,7 @@
     </row>
     <row r="65" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B65" s="6" t="s">
-        <v>274</v>
+        <v>603</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>56</v>
@@ -6541,7 +6854,7 @@
     </row>
     <row r="66" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B66" s="6" t="s">
-        <v>275</v>
+        <v>604</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>54</v>
@@ -6593,7 +6906,7 @@
     </row>
     <row r="67" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B67" s="6" t="s">
-        <v>276</v>
+        <v>605</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>48</v>
@@ -6645,7 +6958,7 @@
     </row>
     <row r="68" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B68" s="6" t="s">
-        <v>277</v>
+        <v>606</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>48</v>
@@ -6697,7 +7010,7 @@
     </row>
     <row r="69" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B69" s="6" t="s">
-        <v>278</v>
+        <v>607</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>48</v>
@@ -6749,7 +7062,7 @@
     </row>
     <row r="70" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B70" s="6" t="s">
-        <v>279</v>
+        <v>608</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>48</v>
@@ -6801,7 +7114,7 @@
     </row>
     <row r="71" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B71" s="6" t="s">
-        <v>280</v>
+        <v>609</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>48</v>
@@ -6853,7 +7166,7 @@
     </row>
     <row r="72" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B72" s="6" t="s">
-        <v>281</v>
+        <v>610</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>48</v>
@@ -6905,7 +7218,7 @@
     </row>
     <row r="73" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B73" s="6" t="s">
-        <v>282</v>
+        <v>611</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>48</v>
@@ -6957,7 +7270,7 @@
     </row>
     <row r="74" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B74" s="6" t="s">
-        <v>283</v>
+        <v>612</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>48</v>
@@ -7009,7 +7322,7 @@
     </row>
     <row r="75" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B75" s="6" t="s">
-        <v>284</v>
+        <v>613</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>48</v>
@@ -7061,7 +7374,7 @@
     </row>
     <row r="76" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B76" s="6" t="s">
-        <v>285</v>
+        <v>614</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>58</v>
@@ -7113,7 +7426,7 @@
     </row>
     <row r="77" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B77" s="6" t="s">
-        <v>286</v>
+        <v>615</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>58</v>
@@ -7165,7 +7478,7 @@
     </row>
     <row r="78" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B78" s="6" t="s">
-        <v>287</v>
+        <v>616</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>65</v>
@@ -7217,7 +7530,7 @@
     </row>
     <row r="79" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B79" s="6" t="s">
-        <v>288</v>
+        <v>617</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>74</v>
@@ -7269,7 +7582,7 @@
     </row>
     <row r="80" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B80" s="6" t="s">
-        <v>289</v>
+        <v>618</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>74</v>
@@ -7321,7 +7634,7 @@
     </row>
     <row r="81" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B81" s="6" t="s">
-        <v>290</v>
+        <v>619</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>58</v>
@@ -7373,7 +7686,7 @@
     </row>
     <row r="82" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B82" s="6" t="s">
-        <v>291</v>
+        <v>620</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>58</v>
@@ -7425,7 +7738,7 @@
     </row>
     <row r="83" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B83" s="6" t="s">
-        <v>292</v>
+        <v>621</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>58</v>
@@ -7477,7 +7790,7 @@
     </row>
     <row r="84" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B84" s="6" t="s">
-        <v>293</v>
+        <v>622</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>58</v>
@@ -7529,7 +7842,7 @@
     </row>
     <row r="85" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B85" s="6" t="s">
-        <v>294</v>
+        <v>623</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>58</v>
@@ -7581,7 +7894,7 @@
     </row>
     <row r="86" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B86" s="6" t="s">
-        <v>295</v>
+        <v>624</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>48</v>
@@ -7633,7 +7946,7 @@
     </row>
     <row r="87" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B87" s="6" t="s">
-        <v>296</v>
+        <v>625</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>48</v>
@@ -7685,7 +7998,7 @@
     </row>
     <row r="88" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B88" s="6" t="s">
-        <v>297</v>
+        <v>626</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>57</v>
@@ -7737,7 +8050,7 @@
     </row>
     <row r="89" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B89" s="6" t="s">
-        <v>298</v>
+        <v>627</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>57</v>
@@ -7789,7 +8102,7 @@
     </row>
     <row r="90" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B90" s="6" t="s">
-        <v>299</v>
+        <v>628</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>57</v>
@@ -7841,7 +8154,7 @@
     </row>
     <row r="91" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B91" s="6" t="s">
-        <v>300</v>
+        <v>629</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>57</v>
@@ -7893,7 +8206,7 @@
     </row>
     <row r="92" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B92" s="6" t="s">
-        <v>301</v>
+        <v>630</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>57</v>
@@ -7945,7 +8258,7 @@
     </row>
     <row r="93" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B93" s="6" t="s">
-        <v>302</v>
+        <v>631</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>57</v>
@@ -7997,7 +8310,7 @@
     </row>
     <row r="94" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B94" s="6" t="s">
-        <v>303</v>
+        <v>632</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>57</v>
@@ -8049,7 +8362,7 @@
     </row>
     <row r="95" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B95" s="6" t="s">
-        <v>304</v>
+        <v>633</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>57</v>
@@ -8101,7 +8414,7 @@
     </row>
     <row r="96" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B96" s="6" t="s">
-        <v>305</v>
+        <v>634</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>57</v>
@@ -8153,7 +8466,7 @@
     </row>
     <row r="97" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B97" s="6" t="s">
-        <v>306</v>
+        <v>635</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>57</v>

</xml_diff>